<commit_message>
Addition of .TXT mapping and scoring files.
</commit_message>
<xml_diff>
--- a/Snplists/T1D_GRS67/T1D_GRS67_1000G_nopalin_pos_hg19.xlsx
+++ b/Snplists/T1D_GRS67/T1D_GRS67_1000G_nopalin_pos_hg19.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{FCAE6DCA-AE44-0448-B6F3-3E1A9A87198D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D0B45911-9B4A-5648-9D52-A8A2C0BCB000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16500" xr2:uid="{790D5DEB-C308-234D-BB35-18DFB1DC5B15}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16500" xr2:uid="{790D5DEB-C308-234D-BB35-18DFB1DC5B15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -952,7 +952,7 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed 11: on the first non-HLA rs
</commit_message>
<xml_diff>
--- a/Snplists/T1D_GRS67/T1D_GRS67_1000G_nopalin_pos_hg19.xlsx
+++ b/Snplists/T1D_GRS67/T1D_GRS67_1000G_nopalin_pos_hg19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/s_sharp_exeter_ac_uk/Documents/LIVE/hla-prs-toolkit/Snplists/T1D_GRS67/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\programming\hla-prs-toolkit\Snplists\T1D_GRS67\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{FCAE6DCA-AE44-0448-B6F3-3E1A9A87198D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D0B45911-9B4A-5648-9D52-A8A2C0BCB000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD8B978-AFC2-4238-AC76-456904907FB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16500" xr2:uid="{790D5DEB-C308-234D-BB35-18DFB1DC5B15}"/>
+    <workbookView xWindow="-19310" yWindow="-80" windowWidth="19420" windowHeight="11020" xr2:uid="{790D5DEB-C308-234D-BB35-18DFB1DC5B15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="180">
   <si>
     <t>STRAND</t>
   </si>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t>10:6129643</t>
+  </si>
+  <si>
+    <t>11:2181060</t>
   </si>
 </sst>
 </file>
@@ -951,11 +954,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2936C92A-3A1B-4C43-81CA-C5EF6A570C1B}">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -967,7 +970,7 @@
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -999,7 +1002,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>150</v>
       </c>
@@ -1032,7 +1035,7 @@
       </c>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
@@ -1065,7 +1068,7 @@
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>152</v>
       </c>
@@ -1100,7 +1103,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>153</v>
       </c>
@@ -1135,7 +1138,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>154</v>
       </c>
@@ -1170,7 +1173,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>155</v>
       </c>
@@ -1205,7 +1208,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>156</v>
       </c>
@@ -1240,7 +1243,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>157</v>
       </c>
@@ -1275,7 +1278,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>158</v>
       </c>
@@ -1310,7 +1313,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>159</v>
       </c>
@@ -1345,7 +1348,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>164</v>
       </c>
@@ -1380,7 +1383,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>161</v>
       </c>
@@ -1415,7 +1418,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>165</v>
       </c>
@@ -1450,7 +1453,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>160</v>
       </c>
@@ -1485,7 +1488,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1520,7 +1523,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1555,7 +1558,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1590,7 +1593,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1625,7 +1628,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1660,7 +1663,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1695,7 +1698,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1730,7 +1733,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1765,7 +1768,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1800,7 +1803,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1835,7 +1838,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1870,7 +1873,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1905,7 +1908,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1940,7 +1943,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1975,7 +1978,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -2010,7 +2013,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -2045,7 +2048,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -2109,7 +2112,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
@@ -2173,7 +2176,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -2205,7 +2208,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>75</v>
       </c>
@@ -2221,8 +2224,8 @@
       <c r="E37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="1">
-        <v>2181060</v>
+      <c r="F37" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>78</v>
@@ -2237,7 +2240,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>75</v>
       </c>
@@ -2269,7 +2272,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>75</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>75</v>
       </c>
@@ -2333,7 +2336,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>75</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>75</v>
       </c>
@@ -2397,7 +2400,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
@@ -2429,7 +2432,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>75</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>75</v>
       </c>
@@ -2493,7 +2496,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>75</v>
       </c>
@@ -2525,7 +2528,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>75</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>75</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>75</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>75</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
@@ -2685,7 +2688,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>75</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>75</v>
       </c>
@@ -2749,7 +2752,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>75</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>75</v>
       </c>
@@ -2813,7 +2816,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>75</v>
       </c>
@@ -2845,7 +2848,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>75</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>75</v>
       </c>
@@ -2909,7 +2912,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>75</v>
       </c>
@@ -2941,7 +2944,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>75</v>
       </c>
@@ -2973,7 +2976,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
@@ -3005,7 +3008,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>75</v>
       </c>
@@ -3037,7 +3040,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>75</v>
       </c>
@@ -3069,7 +3072,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>75</v>
       </c>
@@ -3101,7 +3104,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>75</v>
       </c>
@@ -3133,7 +3136,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>75</v>
       </c>
@@ -3165,7 +3168,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>75</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>75</v>
       </c>

</xml_diff>